<commit_message>
Fixed CSP header documentation, also further explained encoding for gyroscope, ADC1 and ADC2 (in ADCS module).
</commit_message>
<xml_diff>
--- a/docs/Beacon_Package_Data.xlsx
+++ b/docs/Beacon_Package_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dalvarez.AEROBOTS\Documents\UVG\repos\gr-quetzal1\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A488DFD-8124-4748-8E58-F070D5D07A44}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EC91ED1-3475-46CA-8381-28A487C1ACA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-5835" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-5835" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HDLC + AX.25 Frame Structure" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="264">
   <si>
     <t>Package</t>
   </si>
@@ -448,9 +448,6 @@
     <t>0.78 deg/bit</t>
   </si>
   <si>
-    <t>Gyroscope is set to return values in deg/sec.</t>
-  </si>
-  <si>
     <t>Magnetometer</t>
   </si>
   <si>
@@ -473,9 +470,6 @@
   </si>
   <si>
     <t>12.9 mV/bit</t>
-  </si>
-  <si>
-    <t>Maximum value 3.3V with an increase of 3.3V/255 (0.0129V) per bit</t>
   </si>
   <si>
     <t>ADC2</t>
@@ -748,15 +742,6 @@
     <t>50 BYTES (repeating)</t>
   </si>
   <si>
-    <t>SOURCE = 0</t>
-  </si>
-  <si>
-    <t>SOURCE PORT = 2</t>
-  </si>
-  <si>
-    <t>RDP = 1</t>
-  </si>
-  <si>
     <t>Signed char (1 byte) transmitted directly, no encoding</t>
   </si>
   <si>
@@ -772,18 +757,7 @@
     <t>(CSP HEADER) 4 BYTES</t>
   </si>
   <si>
-    <t>DESTINATION = 
-usually 6 or 7</t>
-  </si>
-  <si>
-    <t>DESTINATION
-PORT = varies</t>
-  </si>
-  <si>
     <t>Communication success (S: 0x53) Error (E: 0x45 )</t>
-  </si>
-  <si>
-    <t>bits = 1.275 * gyro + 127.5</t>
   </si>
   <si>
     <t>bits = (8192/325) * magneto + 65536/2 for x, y axes
@@ -827,6 +801,35 @@
   </si>
   <si>
     <t>Maximum of 65,535 resets (0-2^16)</t>
+  </si>
+  <si>
+    <t>SOURCE = 1</t>
+  </si>
+  <si>
+    <t>DESTINATION = 0</t>
+  </si>
+  <si>
+    <t>DESTINATION
+PORT = 9</t>
+  </si>
+  <si>
+    <t>SOURCE PORT 
+= varies</t>
+  </si>
+  <si>
+    <t>RDP = 0</t>
+  </si>
+  <si>
+    <t>bits = 1.275 * gyro_axis + 127.5</t>
+  </si>
+  <si>
+    <t>Gyroscope is set to return values in deg/sec. 1 byte per axis equals 3 bytes total.</t>
+  </si>
+  <si>
+    <t>Connected to 6 photodiodes, one on each solar panel face, one byte per photodiode.</t>
+  </si>
+  <si>
+    <t>Connected to another 6 photodiodes, one on each solar panel face, one byte per photodiode.</t>
   </si>
 </sst>
 </file>
@@ -1575,7 +1578,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="170">
+  <cellXfs count="171">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2042,6 +2045,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2361,23 +2367,23 @@
   </sheetPr>
   <dimension ref="A1:S15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="N8" sqref="N8:N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="123" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B1" s="124"/>
       <c r="C1" s="123" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D1" s="124"/>
       <c r="E1" s="123" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="F1" s="124"/>
       <c r="G1" s="124"/>
@@ -2390,11 +2396,11 @@
       <c r="N1" s="124"/>
       <c r="O1" s="124"/>
       <c r="P1" s="123" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="Q1" s="124"/>
       <c r="R1" s="123" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="S1" s="124"/>
     </row>
@@ -2526,48 +2532,48 @@
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="124" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B8" s="124"/>
       <c r="C8" s="102"/>
       <c r="D8" s="102"/>
       <c r="E8" s="125" t="s">
+        <v>229</v>
+      </c>
+      <c r="F8" s="125" t="s">
+        <v>255</v>
+      </c>
+      <c r="G8" s="126" t="s">
+        <v>256</v>
+      </c>
+      <c r="H8" s="126" t="s">
+        <v>257</v>
+      </c>
+      <c r="I8" s="126" t="s">
+        <v>258</v>
+      </c>
+      <c r="J8" s="125" t="s">
+        <v>230</v>
+      </c>
+      <c r="K8" s="125" t="s">
         <v>231</v>
       </c>
-      <c r="F8" s="125" t="s">
-        <v>237</v>
-      </c>
-      <c r="G8" s="126" t="s">
-        <v>245</v>
-      </c>
-      <c r="H8" s="126" t="s">
-        <v>246</v>
-      </c>
-      <c r="I8" s="125" t="s">
-        <v>238</v>
-      </c>
-      <c r="J8" s="125" t="s">
+      <c r="L8" s="125" t="s">
         <v>232</v>
       </c>
-      <c r="K8" s="125" t="s">
+      <c r="M8" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="N8" s="125" t="s">
         <v>233</v>
       </c>
-      <c r="L8" s="125" t="s">
-        <v>234</v>
-      </c>
-      <c r="M8" s="125" t="s">
-        <v>239</v>
-      </c>
-      <c r="N8" s="125" t="s">
-        <v>235</v>
-      </c>
       <c r="O8" s="126" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="P8" s="102"/>
       <c r="Q8" s="101"/>
       <c r="R8" s="127" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="S8" s="128"/>
     </row>
@@ -2699,15 +2705,15 @@
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="133" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B15" s="133"/>
       <c r="C15" s="134" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D15" s="133"/>
       <c r="E15" s="133" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="F15" s="133"/>
       <c r="G15" s="133"/>
@@ -2719,14 +2725,14 @@
       <c r="M15" s="133"/>
       <c r="N15" s="133"/>
       <c r="O15" s="105" t="s">
+        <v>223</v>
+      </c>
+      <c r="P15" s="133" t="s">
         <v>225</v>
-      </c>
-      <c r="P15" s="133" t="s">
-        <v>227</v>
       </c>
       <c r="Q15" s="133"/>
       <c r="R15" s="133" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="S15" s="133"/>
     </row>
@@ -2765,11 +2771,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AG1031"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="4" ySplit="3" topLeftCell="E19" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="4" ySplit="3" topLeftCell="E24" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C86" sqref="C86"/>
+      <selection pane="bottomRight" activeCell="N39" sqref="N39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3136,7 +3142,7 @@
       <c r="L8" s="23"/>
       <c r="M8" s="21"/>
       <c r="N8" s="120" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="O8" s="16"/>
       <c r="P8" s="16"/>
@@ -3179,7 +3185,7 @@
       <c r="L9" s="23"/>
       <c r="M9" s="21"/>
       <c r="N9" s="26" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="O9" s="16"/>
       <c r="P9" s="16"/>
@@ -3265,7 +3271,7 @@
       <c r="L11" s="28"/>
       <c r="M11" s="29"/>
       <c r="N11" s="121" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="O11" s="16"/>
       <c r="P11" s="16"/>
@@ -3308,7 +3314,7 @@
       <c r="L12" s="28"/>
       <c r="M12" s="29"/>
       <c r="N12" s="121" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="O12" s="16"/>
       <c r="P12" s="16"/>
@@ -3351,7 +3357,7 @@
       <c r="L13" s="28"/>
       <c r="M13" s="29"/>
       <c r="N13" s="121" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="O13" s="16"/>
       <c r="P13" s="16"/>
@@ -3394,7 +3400,7 @@
       <c r="L14" s="28"/>
       <c r="M14" s="29"/>
       <c r="N14" s="121" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="O14" s="16"/>
       <c r="P14" s="16"/>
@@ -3437,7 +3443,7 @@
       <c r="L15" s="28"/>
       <c r="M15" s="29"/>
       <c r="N15" s="121" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="O15" s="16"/>
       <c r="P15" s="16"/>
@@ -3481,7 +3487,7 @@
       <c r="L16" s="31"/>
       <c r="M16" s="32"/>
       <c r="N16" s="122" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="O16" s="16"/>
       <c r="P16" s="16"/>
@@ -4680,11 +4686,11 @@
         <v>123</v>
       </c>
       <c r="L37" s="108" t="s">
-        <v>248</v>
+        <v>260</v>
       </c>
       <c r="M37" s="55"/>
-      <c r="N37" s="56" t="s">
-        <v>137</v>
+      <c r="N37" s="170" t="s">
+        <v>261</v>
       </c>
       <c r="O37" s="1"/>
       <c r="P37" s="1"/>
@@ -4711,7 +4717,7 @@
       <c r="B38" s="142"/>
       <c r="C38" s="140"/>
       <c r="D38" s="33" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E38" s="34">
         <v>48</v>
@@ -4721,26 +4727,26 @@
         <v>6</v>
       </c>
       <c r="G38" s="45" t="s">
+        <v>138</v>
+      </c>
+      <c r="H38" s="45" t="s">
+        <v>138</v>
+      </c>
+      <c r="I38" s="34" t="s">
         <v>139</v>
       </c>
-      <c r="H38" s="45" t="s">
-        <v>139</v>
-      </c>
-      <c r="I38" s="34" t="s">
+      <c r="J38" s="34" t="s">
         <v>140</v>
-      </c>
-      <c r="J38" s="34" t="s">
-        <v>141</v>
       </c>
       <c r="K38" s="34" t="s">
         <v>123</v>
       </c>
       <c r="L38" s="109" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="M38" s="57"/>
       <c r="N38" s="39" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="O38" s="1"/>
       <c r="P38" s="1"/>
@@ -4767,7 +4773,7 @@
       <c r="B39" s="142"/>
       <c r="C39" s="140"/>
       <c r="D39" s="38" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E39" s="58">
         <v>48</v>
@@ -4777,26 +4783,26 @@
         <v>6</v>
       </c>
       <c r="G39" s="34" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H39" s="34" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I39" s="34" t="s">
         <v>135</v>
       </c>
       <c r="J39" s="34" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="K39" s="34" t="s">
         <v>123</v>
       </c>
       <c r="L39" s="59" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="M39" s="60"/>
       <c r="N39" s="61" t="s">
-        <v>146</v>
+        <v>262</v>
       </c>
       <c r="O39" s="1"/>
       <c r="P39" s="1"/>
@@ -4823,7 +4829,7 @@
       <c r="B40" s="142"/>
       <c r="C40" s="150"/>
       <c r="D40" s="38" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E40" s="58">
         <v>48</v>
@@ -4833,26 +4839,26 @@
         <v>6</v>
       </c>
       <c r="G40" s="34" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H40" s="34" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I40" s="34" t="s">
         <v>135</v>
       </c>
       <c r="J40" s="34" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="K40" s="34" t="s">
         <v>123</v>
       </c>
       <c r="L40" s="59" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="M40" s="60"/>
       <c r="N40" s="61" t="s">
-        <v>146</v>
+        <v>263</v>
       </c>
       <c r="O40" s="1"/>
       <c r="P40" s="1"/>
@@ -4878,10 +4884,10 @@
       <c r="A41" s="1"/>
       <c r="B41" s="142"/>
       <c r="C41" s="34" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D41" s="38" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E41" s="34">
         <v>8</v>
@@ -4891,26 +4897,26 @@
         <v>1</v>
       </c>
       <c r="G41" s="34" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="H41" s="34" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="I41" s="58" t="s">
         <v>135</v>
       </c>
       <c r="J41" s="34" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="K41" s="34" t="s">
         <v>123</v>
       </c>
       <c r="L41" s="111" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="M41" s="62"/>
       <c r="N41" s="106" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="O41" s="1"/>
       <c r="P41" s="1"/>
@@ -4936,7 +4942,7 @@
       <c r="A42" s="1"/>
       <c r="B42" s="142"/>
       <c r="C42" s="38" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D42" s="33" t="s">
         <v>38</v>
@@ -4949,26 +4955,26 @@
         <v>2</v>
       </c>
       <c r="G42" s="34" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="H42" s="34" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I42" s="110" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="J42" s="110" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="K42" s="34" t="s">
         <v>123</v>
       </c>
       <c r="L42" s="111" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="M42" s="62"/>
       <c r="N42" s="46" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="O42" s="1"/>
       <c r="P42" s="1"/>
@@ -4994,10 +5000,10 @@
       <c r="A43" s="1"/>
       <c r="B43" s="142"/>
       <c r="C43" s="154" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D43" s="38" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E43" s="157">
         <v>8</v>
@@ -5009,18 +5015,18 @@
       <c r="G43" s="64"/>
       <c r="H43" s="44"/>
       <c r="I43" s="34" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="J43" s="44"/>
       <c r="K43" s="34">
         <v>0</v>
       </c>
       <c r="L43" s="111" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="M43" s="62"/>
       <c r="N43" s="39" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="O43" s="1"/>
       <c r="P43" s="1"/>
@@ -5047,25 +5053,25 @@
       <c r="B44" s="142"/>
       <c r="C44" s="140"/>
       <c r="D44" s="38" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E44" s="140"/>
       <c r="F44" s="140"/>
       <c r="G44" s="65"/>
       <c r="H44" s="44"/>
       <c r="I44" s="34" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="J44" s="44"/>
       <c r="K44" s="34">
         <v>0</v>
       </c>
       <c r="L44" s="111" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="M44" s="62"/>
       <c r="N44" s="39" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="O44" s="1"/>
       <c r="P44" s="1"/>
@@ -5092,25 +5098,25 @@
       <c r="B45" s="142"/>
       <c r="C45" s="140"/>
       <c r="D45" s="38" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E45" s="140"/>
       <c r="F45" s="140"/>
       <c r="G45" s="65"/>
       <c r="H45" s="44"/>
       <c r="I45" s="34" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="J45" s="44"/>
       <c r="K45" s="34">
         <v>0</v>
       </c>
       <c r="L45" s="111" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="M45" s="62"/>
       <c r="N45" s="39" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="O45" s="1"/>
       <c r="P45" s="1"/>
@@ -5137,25 +5143,25 @@
       <c r="B46" s="136"/>
       <c r="C46" s="155"/>
       <c r="D46" s="43" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E46" s="155"/>
       <c r="F46" s="155"/>
       <c r="G46" s="66"/>
       <c r="H46" s="67"/>
       <c r="I46" s="63" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="J46" s="67"/>
       <c r="K46" s="63">
         <v>0</v>
       </c>
       <c r="L46" s="115" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="M46" s="113"/>
       <c r="N46" s="114" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="O46" s="1"/>
       <c r="P46" s="1"/>
@@ -5180,10 +5186,10 @@
     <row r="47" spans="1:33" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="1"/>
       <c r="B47" s="68" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C47" s="137" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D47" s="138"/>
       <c r="E47" s="69">
@@ -5201,7 +5207,7 @@
       <c r="L47" s="70"/>
       <c r="M47" s="112"/>
       <c r="N47" s="79" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="O47" s="1"/>
       <c r="P47" s="1"/>
@@ -5226,13 +5232,13 @@
     <row r="48" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="135" t="s">
+        <v>165</v>
+      </c>
+      <c r="C48" s="72" t="s">
+        <v>166</v>
+      </c>
+      <c r="D48" s="54" t="s">
         <v>167</v>
-      </c>
-      <c r="C48" s="72" t="s">
-        <v>168</v>
-      </c>
-      <c r="D48" s="54" t="s">
-        <v>169</v>
       </c>
       <c r="E48" s="53">
         <v>8</v>
@@ -5248,7 +5254,7 @@
       <c r="L48" s="73"/>
       <c r="M48" s="74"/>
       <c r="N48" s="56" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="O48" s="1"/>
       <c r="P48" s="1"/>
@@ -5274,10 +5280,10 @@
       <c r="A49" s="1"/>
       <c r="B49" s="136"/>
       <c r="C49" s="75" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D49" s="76" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E49" s="77">
         <v>16</v>
@@ -5294,7 +5300,7 @@
       <c r="L49" s="76"/>
       <c r="M49" s="78"/>
       <c r="N49" s="79" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="O49" s="1"/>
       <c r="P49" s="1"/>
@@ -5319,10 +5325,10 @@
     <row r="50" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="141" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C50" s="139" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D50" s="140"/>
       <c r="E50" s="80">
@@ -5363,7 +5369,7 @@
       <c r="A51" s="1"/>
       <c r="B51" s="142"/>
       <c r="C51" s="139" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D51" s="140"/>
       <c r="E51" s="80">
@@ -5404,7 +5410,7 @@
       <c r="A52" s="1"/>
       <c r="B52" s="142"/>
       <c r="C52" s="139" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D52" s="140"/>
       <c r="E52" s="80">
@@ -5445,7 +5451,7 @@
       <c r="A53" s="1"/>
       <c r="B53" s="142"/>
       <c r="C53" s="139" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D53" s="140"/>
       <c r="E53" s="80">
@@ -5486,7 +5492,7 @@
       <c r="A54" s="1"/>
       <c r="B54" s="142"/>
       <c r="C54" s="139" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D54" s="140"/>
       <c r="E54" s="80">
@@ -5527,7 +5533,7 @@
       <c r="A55" s="1"/>
       <c r="B55" s="142"/>
       <c r="C55" s="139" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D55" s="140"/>
       <c r="E55" s="80">
@@ -5568,7 +5574,7 @@
       <c r="A56" s="1"/>
       <c r="B56" s="142"/>
       <c r="C56" s="139" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D56" s="140"/>
       <c r="E56" s="80">
@@ -5609,7 +5615,7 @@
       <c r="A57" s="1"/>
       <c r="B57" s="142"/>
       <c r="C57" s="139" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D57" s="140"/>
       <c r="E57" s="80">
@@ -5650,7 +5656,7 @@
       <c r="A58" s="1"/>
       <c r="B58" s="142"/>
       <c r="C58" s="139" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D58" s="140"/>
       <c r="E58" s="80">
@@ -5691,7 +5697,7 @@
       <c r="A59" s="1"/>
       <c r="B59" s="142"/>
       <c r="C59" s="139" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D59" s="140"/>
       <c r="E59" s="80">
@@ -5732,7 +5738,7 @@
       <c r="A60" s="1"/>
       <c r="B60" s="142"/>
       <c r="C60" s="139" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D60" s="140"/>
       <c r="E60" s="80">
@@ -5773,7 +5779,7 @@
       <c r="A61" s="1"/>
       <c r="B61" s="142"/>
       <c r="C61" s="139" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D61" s="140"/>
       <c r="E61" s="80">
@@ -5814,7 +5820,7 @@
       <c r="A62" s="1"/>
       <c r="B62" s="142"/>
       <c r="C62" s="139" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D62" s="140"/>
       <c r="E62" s="80">
@@ -5855,7 +5861,7 @@
       <c r="A63" s="1"/>
       <c r="B63" s="142"/>
       <c r="C63" s="139" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D63" s="140"/>
       <c r="E63" s="80">
@@ -5896,7 +5902,7 @@
       <c r="A64" s="1"/>
       <c r="B64" s="142"/>
       <c r="C64" s="139" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D64" s="140"/>
       <c r="E64" s="80">
@@ -5937,7 +5943,7 @@
       <c r="A65" s="1"/>
       <c r="B65" s="142"/>
       <c r="C65" s="139" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D65" s="140"/>
       <c r="E65" s="80">
@@ -5978,7 +5984,7 @@
       <c r="A66" s="1"/>
       <c r="B66" s="142"/>
       <c r="C66" s="139" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D66" s="140"/>
       <c r="E66" s="80">
@@ -6019,7 +6025,7 @@
       <c r="A67" s="1"/>
       <c r="B67" s="142"/>
       <c r="C67" s="139" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D67" s="140"/>
       <c r="E67" s="80">
@@ -6060,7 +6066,7 @@
       <c r="A68" s="1"/>
       <c r="B68" s="142"/>
       <c r="C68" s="139" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D68" s="140"/>
       <c r="E68" s="80">
@@ -6101,7 +6107,7 @@
       <c r="A69" s="1"/>
       <c r="B69" s="142"/>
       <c r="C69" s="139" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D69" s="140"/>
       <c r="E69" s="80">
@@ -6142,7 +6148,7 @@
       <c r="A70" s="1"/>
       <c r="B70" s="142"/>
       <c r="C70" s="139" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D70" s="140"/>
       <c r="E70" s="80">
@@ -6183,7 +6189,7 @@
       <c r="A71" s="1"/>
       <c r="B71" s="136"/>
       <c r="C71" s="139" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D71" s="140"/>
       <c r="E71" s="80">
@@ -6223,7 +6229,7 @@
     <row r="72" spans="1:33" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="1"/>
       <c r="B72" s="85" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C72" s="86"/>
       <c r="D72" s="87"/>
@@ -6241,7 +6247,7 @@
       <c r="L72" s="71"/>
       <c r="M72" s="71"/>
       <c r="N72" s="107" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="O72" s="1"/>
       <c r="P72" s="1"/>
@@ -6266,7 +6272,7 @@
     <row r="73" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
       <c r="B73" s="91" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C73" s="92">
         <f>SUM(E4:E72)</f>
@@ -6383,7 +6389,7 @@
     <row r="76" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
       <c r="B76" s="95" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C76" s="4"/>
       <c r="D76" s="1"/>
@@ -6420,16 +6426,16 @@
     <row r="77" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
       <c r="B77" s="60" t="s">
+        <v>197</v>
+      </c>
+      <c r="C77" s="25" t="s">
+        <v>198</v>
+      </c>
+      <c r="D77" s="60" t="s">
         <v>199</v>
       </c>
-      <c r="C77" s="25" t="s">
+      <c r="E77" s="143" t="s">
         <v>200</v>
-      </c>
-      <c r="D77" s="60" t="s">
-        <v>201</v>
-      </c>
-      <c r="E77" s="143" t="s">
-        <v>202</v>
       </c>
       <c r="F77" s="144"/>
       <c r="G77" s="144"/>
@@ -6437,7 +6443,7 @@
       <c r="I77" s="144"/>
       <c r="J77" s="145"/>
       <c r="K77" s="143" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="L77" s="145"/>
       <c r="M77" s="3"/>
@@ -6468,13 +6474,13 @@
         <v>253</v>
       </c>
       <c r="C78" s="25" t="s">
+        <v>202</v>
+      </c>
+      <c r="D78" s="60" t="s">
+        <v>203</v>
+      </c>
+      <c r="E78" s="143" t="s">
         <v>204</v>
-      </c>
-      <c r="D78" s="60" t="s">
-        <v>205</v>
-      </c>
-      <c r="E78" s="143" t="s">
-        <v>206</v>
       </c>
       <c r="F78" s="144"/>
       <c r="G78" s="144"/>
@@ -6482,7 +6488,7 @@
       <c r="I78" s="144"/>
       <c r="J78" s="145"/>
       <c r="K78" s="146" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="L78" s="147"/>
       <c r="M78" s="96"/>
@@ -6513,13 +6519,13 @@
         <v>254</v>
       </c>
       <c r="C79" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="D79" s="60" t="s">
+        <v>207</v>
+      </c>
+      <c r="E79" s="143" t="s">
         <v>208</v>
-      </c>
-      <c r="D79" s="60" t="s">
-        <v>209</v>
-      </c>
-      <c r="E79" s="143" t="s">
-        <v>210</v>
       </c>
       <c r="F79" s="144"/>
       <c r="G79" s="144"/>
@@ -6556,13 +6562,13 @@
         <v>255</v>
       </c>
       <c r="C80" s="25" t="s">
+        <v>209</v>
+      </c>
+      <c r="D80" s="60" t="s">
+        <v>210</v>
+      </c>
+      <c r="E80" s="143" t="s">
         <v>211</v>
-      </c>
-      <c r="D80" s="60" t="s">
-        <v>212</v>
-      </c>
-      <c r="E80" s="143" t="s">
-        <v>213</v>
       </c>
       <c r="F80" s="144"/>
       <c r="G80" s="144"/>
@@ -6599,13 +6605,13 @@
         <v>4093</v>
       </c>
       <c r="C81" s="25" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D81" s="60" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E81" s="143" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="F81" s="144"/>
       <c r="G81" s="144"/>
@@ -6642,13 +6648,13 @@
         <v>4094</v>
       </c>
       <c r="C82" s="25" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D82" s="60" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E82" s="143" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F82" s="144"/>
       <c r="G82" s="144"/>
@@ -6685,13 +6691,13 @@
         <v>4095</v>
       </c>
       <c r="C83" s="25" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D83" s="60" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E83" s="143" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="F83" s="144"/>
       <c r="G83" s="144"/>
@@ -6754,7 +6760,7 @@
     <row r="85" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
       <c r="B85" s="99" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C85" s="100"/>
       <c r="D85" s="97"/>

</xml_diff>

<commit_message>
Revert "Fixed CSP header documentation, also further explained encoding for gyroscope, ADC1 and ADC2 (in ADCS module)."
This reverts commit e47aab5a5c7cbf795efe4e1218783139c5675b41.
</commit_message>
<xml_diff>
--- a/docs/Beacon_Package_Data.xlsx
+++ b/docs/Beacon_Package_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dalvarez.AEROBOTS\Documents\UVG\repos\gr-quetzal1\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EC91ED1-3475-46CA-8381-28A487C1ACA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A488DFD-8124-4748-8E58-F070D5D07A44}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-5835" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-5835" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HDLC + AX.25 Frame Structure" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="263">
   <si>
     <t>Package</t>
   </si>
@@ -448,6 +448,9 @@
     <t>0.78 deg/bit</t>
   </si>
   <si>
+    <t>Gyroscope is set to return values in deg/sec.</t>
+  </si>
+  <si>
     <t>Magnetometer</t>
   </si>
   <si>
@@ -470,6 +473,9 @@
   </si>
   <si>
     <t>12.9 mV/bit</t>
+  </si>
+  <si>
+    <t>Maximum value 3.3V with an increase of 3.3V/255 (0.0129V) per bit</t>
   </si>
   <si>
     <t>ADC2</t>
@@ -742,6 +748,15 @@
     <t>50 BYTES (repeating)</t>
   </si>
   <si>
+    <t>SOURCE = 0</t>
+  </si>
+  <si>
+    <t>SOURCE PORT = 2</t>
+  </si>
+  <si>
+    <t>RDP = 1</t>
+  </si>
+  <si>
     <t>Signed char (1 byte) transmitted directly, no encoding</t>
   </si>
   <si>
@@ -757,7 +772,18 @@
     <t>(CSP HEADER) 4 BYTES</t>
   </si>
   <si>
+    <t>DESTINATION = 
+usually 6 or 7</t>
+  </si>
+  <si>
+    <t>DESTINATION
+PORT = varies</t>
+  </si>
+  <si>
     <t>Communication success (S: 0x53) Error (E: 0x45 )</t>
+  </si>
+  <si>
+    <t>bits = 1.275 * gyro + 127.5</t>
   </si>
   <si>
     <t>bits = (8192/325) * magneto + 65536/2 for x, y axes
@@ -801,35 +827,6 @@
   </si>
   <si>
     <t>Maximum of 65,535 resets (0-2^16)</t>
-  </si>
-  <si>
-    <t>SOURCE = 1</t>
-  </si>
-  <si>
-    <t>DESTINATION = 0</t>
-  </si>
-  <si>
-    <t>DESTINATION
-PORT = 9</t>
-  </si>
-  <si>
-    <t>SOURCE PORT 
-= varies</t>
-  </si>
-  <si>
-    <t>RDP = 0</t>
-  </si>
-  <si>
-    <t>bits = 1.275 * gyro_axis + 127.5</t>
-  </si>
-  <si>
-    <t>Gyroscope is set to return values in deg/sec. 1 byte per axis equals 3 bytes total.</t>
-  </si>
-  <si>
-    <t>Connected to 6 photodiodes, one on each solar panel face, one byte per photodiode.</t>
-  </si>
-  <si>
-    <t>Connected to another 6 photodiodes, one on each solar panel face, one byte per photodiode.</t>
   </si>
 </sst>
 </file>
@@ -1578,7 +1575,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="171">
+  <cellXfs count="170">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2045,9 +2042,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2367,23 +2361,23 @@
   </sheetPr>
   <dimension ref="A1:S15"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8:N14"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="123" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="B1" s="124"/>
       <c r="C1" s="123" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="D1" s="124"/>
       <c r="E1" s="123" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="F1" s="124"/>
       <c r="G1" s="124"/>
@@ -2396,11 +2390,11 @@
       <c r="N1" s="124"/>
       <c r="O1" s="124"/>
       <c r="P1" s="123" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="Q1" s="124"/>
       <c r="R1" s="123" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="S1" s="124"/>
     </row>
@@ -2532,48 +2526,48 @@
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="124" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="B8" s="124"/>
       <c r="C8" s="102"/>
       <c r="D8" s="102"/>
       <c r="E8" s="125" t="s">
+        <v>231</v>
+      </c>
+      <c r="F8" s="125" t="s">
+        <v>237</v>
+      </c>
+      <c r="G8" s="126" t="s">
+        <v>245</v>
+      </c>
+      <c r="H8" s="126" t="s">
+        <v>246</v>
+      </c>
+      <c r="I8" s="125" t="s">
+        <v>238</v>
+      </c>
+      <c r="J8" s="125" t="s">
+        <v>232</v>
+      </c>
+      <c r="K8" s="125" t="s">
+        <v>233</v>
+      </c>
+      <c r="L8" s="125" t="s">
+        <v>234</v>
+      </c>
+      <c r="M8" s="125" t="s">
+        <v>239</v>
+      </c>
+      <c r="N8" s="125" t="s">
+        <v>235</v>
+      </c>
+      <c r="O8" s="126" t="s">
         <v>229</v>
-      </c>
-      <c r="F8" s="125" t="s">
-        <v>255</v>
-      </c>
-      <c r="G8" s="126" t="s">
-        <v>256</v>
-      </c>
-      <c r="H8" s="126" t="s">
-        <v>257</v>
-      </c>
-      <c r="I8" s="126" t="s">
-        <v>258</v>
-      </c>
-      <c r="J8" s="125" t="s">
-        <v>230</v>
-      </c>
-      <c r="K8" s="125" t="s">
-        <v>231</v>
-      </c>
-      <c r="L8" s="125" t="s">
-        <v>232</v>
-      </c>
-      <c r="M8" s="125" t="s">
-        <v>259</v>
-      </c>
-      <c r="N8" s="125" t="s">
-        <v>233</v>
-      </c>
-      <c r="O8" s="126" t="s">
-        <v>227</v>
       </c>
       <c r="P8" s="102"/>
       <c r="Q8" s="101"/>
       <c r="R8" s="127" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="S8" s="128"/>
     </row>
@@ -2705,15 +2699,15 @@
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="133" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="B15" s="133"/>
       <c r="C15" s="134" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="D15" s="133"/>
       <c r="E15" s="133" t="s">
-        <v>239</v>
+        <v>244</v>
       </c>
       <c r="F15" s="133"/>
       <c r="G15" s="133"/>
@@ -2725,14 +2719,14 @@
       <c r="M15" s="133"/>
       <c r="N15" s="133"/>
       <c r="O15" s="105" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="P15" s="133" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="Q15" s="133"/>
       <c r="R15" s="133" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="S15" s="133"/>
     </row>
@@ -2771,11 +2765,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AG1031"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="4" ySplit="3" topLeftCell="E24" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="4" ySplit="3" topLeftCell="E19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="N39" sqref="N39"/>
+      <selection pane="bottomRight" activeCell="C86" sqref="C86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3142,7 +3136,7 @@
       <c r="L8" s="23"/>
       <c r="M8" s="21"/>
       <c r="N8" s="120" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="O8" s="16"/>
       <c r="P8" s="16"/>
@@ -3185,7 +3179,7 @@
       <c r="L9" s="23"/>
       <c r="M9" s="21"/>
       <c r="N9" s="26" t="s">
-        <v>240</v>
+        <v>247</v>
       </c>
       <c r="O9" s="16"/>
       <c r="P9" s="16"/>
@@ -3271,7 +3265,7 @@
       <c r="L11" s="28"/>
       <c r="M11" s="29"/>
       <c r="N11" s="121" t="s">
-        <v>253</v>
+        <v>261</v>
       </c>
       <c r="O11" s="16"/>
       <c r="P11" s="16"/>
@@ -3314,7 +3308,7 @@
       <c r="L12" s="28"/>
       <c r="M12" s="29"/>
       <c r="N12" s="121" t="s">
-        <v>253</v>
+        <v>261</v>
       </c>
       <c r="O12" s="16"/>
       <c r="P12" s="16"/>
@@ -3357,7 +3351,7 @@
       <c r="L13" s="28"/>
       <c r="M13" s="29"/>
       <c r="N13" s="121" t="s">
-        <v>253</v>
+        <v>261</v>
       </c>
       <c r="O13" s="16"/>
       <c r="P13" s="16"/>
@@ -3400,7 +3394,7 @@
       <c r="L14" s="28"/>
       <c r="M14" s="29"/>
       <c r="N14" s="121" t="s">
-        <v>253</v>
+        <v>261</v>
       </c>
       <c r="O14" s="16"/>
       <c r="P14" s="16"/>
@@ -3443,7 +3437,7 @@
       <c r="L15" s="28"/>
       <c r="M15" s="29"/>
       <c r="N15" s="121" t="s">
-        <v>253</v>
+        <v>261</v>
       </c>
       <c r="O15" s="16"/>
       <c r="P15" s="16"/>
@@ -3487,7 +3481,7 @@
       <c r="L16" s="31"/>
       <c r="M16" s="32"/>
       <c r="N16" s="122" t="s">
-        <v>254</v>
+        <v>262</v>
       </c>
       <c r="O16" s="16"/>
       <c r="P16" s="16"/>
@@ -4686,11 +4680,11 @@
         <v>123</v>
       </c>
       <c r="L37" s="108" t="s">
-        <v>260</v>
+        <v>248</v>
       </c>
       <c r="M37" s="55"/>
-      <c r="N37" s="170" t="s">
-        <v>261</v>
+      <c r="N37" s="56" t="s">
+        <v>137</v>
       </c>
       <c r="O37" s="1"/>
       <c r="P37" s="1"/>
@@ -4717,7 +4711,7 @@
       <c r="B38" s="142"/>
       <c r="C38" s="140"/>
       <c r="D38" s="33" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E38" s="34">
         <v>48</v>
@@ -4727,26 +4721,26 @@
         <v>6</v>
       </c>
       <c r="G38" s="45" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="H38" s="45" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="I38" s="34" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="J38" s="34" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="K38" s="34" t="s">
         <v>123</v>
       </c>
       <c r="L38" s="109" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="M38" s="57"/>
       <c r="N38" s="39" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="O38" s="1"/>
       <c r="P38" s="1"/>
@@ -4773,7 +4767,7 @@
       <c r="B39" s="142"/>
       <c r="C39" s="140"/>
       <c r="D39" s="38" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E39" s="58">
         <v>48</v>
@@ -4783,26 +4777,26 @@
         <v>6</v>
       </c>
       <c r="G39" s="34" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="H39" s="34" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="I39" s="34" t="s">
         <v>135</v>
       </c>
       <c r="J39" s="34" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="K39" s="34" t="s">
         <v>123</v>
       </c>
       <c r="L39" s="59" t="s">
-        <v>242</v>
+        <v>250</v>
       </c>
       <c r="M39" s="60"/>
       <c r="N39" s="61" t="s">
-        <v>262</v>
+        <v>146</v>
       </c>
       <c r="O39" s="1"/>
       <c r="P39" s="1"/>
@@ -4829,7 +4823,7 @@
       <c r="B40" s="142"/>
       <c r="C40" s="150"/>
       <c r="D40" s="38" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E40" s="58">
         <v>48</v>
@@ -4839,26 +4833,26 @@
         <v>6</v>
       </c>
       <c r="G40" s="34" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="H40" s="34" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="I40" s="34" t="s">
         <v>135</v>
       </c>
       <c r="J40" s="34" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="K40" s="34" t="s">
         <v>123</v>
       </c>
       <c r="L40" s="59" t="s">
-        <v>243</v>
+        <v>251</v>
       </c>
       <c r="M40" s="60"/>
       <c r="N40" s="61" t="s">
-        <v>263</v>
+        <v>146</v>
       </c>
       <c r="O40" s="1"/>
       <c r="P40" s="1"/>
@@ -4884,10 +4878,10 @@
       <c r="A41" s="1"/>
       <c r="B41" s="142"/>
       <c r="C41" s="34" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="D41" s="38" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="E41" s="34">
         <v>8</v>
@@ -4897,26 +4891,26 @@
         <v>1</v>
       </c>
       <c r="G41" s="34" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="H41" s="34" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="I41" s="58" t="s">
         <v>135</v>
       </c>
       <c r="J41" s="34" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="K41" s="34" t="s">
         <v>123</v>
       </c>
       <c r="L41" s="111" t="s">
-        <v>245</v>
+        <v>253</v>
       </c>
       <c r="M41" s="62"/>
       <c r="N41" s="106" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="O41" s="1"/>
       <c r="P41" s="1"/>
@@ -4942,7 +4936,7 @@
       <c r="A42" s="1"/>
       <c r="B42" s="142"/>
       <c r="C42" s="38" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="D42" s="33" t="s">
         <v>38</v>
@@ -4955,26 +4949,26 @@
         <v>2</v>
       </c>
       <c r="G42" s="34" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="H42" s="34" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="I42" s="110" t="s">
-        <v>247</v>
+        <v>255</v>
       </c>
       <c r="J42" s="110" t="s">
-        <v>248</v>
+        <v>256</v>
       </c>
       <c r="K42" s="34" t="s">
         <v>123</v>
       </c>
       <c r="L42" s="111" t="s">
-        <v>244</v>
+        <v>252</v>
       </c>
       <c r="M42" s="62"/>
       <c r="N42" s="46" t="s">
-        <v>246</v>
+        <v>254</v>
       </c>
       <c r="O42" s="1"/>
       <c r="P42" s="1"/>
@@ -5000,10 +4994,10 @@
       <c r="A43" s="1"/>
       <c r="B43" s="142"/>
       <c r="C43" s="154" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="D43" s="38" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="E43" s="157">
         <v>8</v>
@@ -5015,18 +5009,18 @@
       <c r="G43" s="64"/>
       <c r="H43" s="44"/>
       <c r="I43" s="34" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="J43" s="44"/>
       <c r="K43" s="34">
         <v>0</v>
       </c>
       <c r="L43" s="111" t="s">
-        <v>249</v>
+        <v>257</v>
       </c>
       <c r="M43" s="62"/>
       <c r="N43" s="39" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="O43" s="1"/>
       <c r="P43" s="1"/>
@@ -5053,25 +5047,25 @@
       <c r="B44" s="142"/>
       <c r="C44" s="140"/>
       <c r="D44" s="38" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="E44" s="140"/>
       <c r="F44" s="140"/>
       <c r="G44" s="65"/>
       <c r="H44" s="44"/>
       <c r="I44" s="34" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="J44" s="44"/>
       <c r="K44" s="34">
         <v>0</v>
       </c>
       <c r="L44" s="111" t="s">
-        <v>250</v>
+        <v>258</v>
       </c>
       <c r="M44" s="62"/>
       <c r="N44" s="39" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="O44" s="1"/>
       <c r="P44" s="1"/>
@@ -5098,25 +5092,25 @@
       <c r="B45" s="142"/>
       <c r="C45" s="140"/>
       <c r="D45" s="38" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="E45" s="140"/>
       <c r="F45" s="140"/>
       <c r="G45" s="65"/>
       <c r="H45" s="44"/>
       <c r="I45" s="34" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="J45" s="44"/>
       <c r="K45" s="34">
         <v>0</v>
       </c>
       <c r="L45" s="111" t="s">
-        <v>251</v>
+        <v>259</v>
       </c>
       <c r="M45" s="62"/>
       <c r="N45" s="39" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="O45" s="1"/>
       <c r="P45" s="1"/>
@@ -5143,25 +5137,25 @@
       <c r="B46" s="136"/>
       <c r="C46" s="155"/>
       <c r="D46" s="43" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="E46" s="155"/>
       <c r="F46" s="155"/>
       <c r="G46" s="66"/>
       <c r="H46" s="67"/>
       <c r="I46" s="63" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="J46" s="67"/>
       <c r="K46" s="63">
         <v>0</v>
       </c>
       <c r="L46" s="115" t="s">
-        <v>252</v>
+        <v>260</v>
       </c>
       <c r="M46" s="113"/>
       <c r="N46" s="114" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="O46" s="1"/>
       <c r="P46" s="1"/>
@@ -5186,10 +5180,10 @@
     <row r="47" spans="1:33" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="1"/>
       <c r="B47" s="68" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="C47" s="137" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="D47" s="138"/>
       <c r="E47" s="69">
@@ -5207,7 +5201,7 @@
       <c r="L47" s="70"/>
       <c r="M47" s="112"/>
       <c r="N47" s="79" t="s">
-        <v>236</v>
+        <v>241</v>
       </c>
       <c r="O47" s="1"/>
       <c r="P47" s="1"/>
@@ -5232,13 +5226,13 @@
     <row r="48" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="135" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C48" s="72" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="D48" s="54" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="E48" s="53">
         <v>8</v>
@@ -5254,7 +5248,7 @@
       <c r="L48" s="73"/>
       <c r="M48" s="74"/>
       <c r="N48" s="56" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="O48" s="1"/>
       <c r="P48" s="1"/>
@@ -5280,10 +5274,10 @@
       <c r="A49" s="1"/>
       <c r="B49" s="136"/>
       <c r="C49" s="75" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="D49" s="76" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="E49" s="77">
         <v>16</v>
@@ -5300,7 +5294,7 @@
       <c r="L49" s="76"/>
       <c r="M49" s="78"/>
       <c r="N49" s="79" t="s">
-        <v>236</v>
+        <v>241</v>
       </c>
       <c r="O49" s="1"/>
       <c r="P49" s="1"/>
@@ -5325,10 +5319,10 @@
     <row r="50" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="141" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="C50" s="139" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="D50" s="140"/>
       <c r="E50" s="80">
@@ -5369,7 +5363,7 @@
       <c r="A51" s="1"/>
       <c r="B51" s="142"/>
       <c r="C51" s="139" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="D51" s="140"/>
       <c r="E51" s="80">
@@ -5410,7 +5404,7 @@
       <c r="A52" s="1"/>
       <c r="B52" s="142"/>
       <c r="C52" s="139" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="D52" s="140"/>
       <c r="E52" s="80">
@@ -5451,7 +5445,7 @@
       <c r="A53" s="1"/>
       <c r="B53" s="142"/>
       <c r="C53" s="139" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="D53" s="140"/>
       <c r="E53" s="80">
@@ -5492,7 +5486,7 @@
       <c r="A54" s="1"/>
       <c r="B54" s="142"/>
       <c r="C54" s="139" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="D54" s="140"/>
       <c r="E54" s="80">
@@ -5533,7 +5527,7 @@
       <c r="A55" s="1"/>
       <c r="B55" s="142"/>
       <c r="C55" s="139" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="D55" s="140"/>
       <c r="E55" s="80">
@@ -5574,7 +5568,7 @@
       <c r="A56" s="1"/>
       <c r="B56" s="142"/>
       <c r="C56" s="139" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="D56" s="140"/>
       <c r="E56" s="80">
@@ -5615,7 +5609,7 @@
       <c r="A57" s="1"/>
       <c r="B57" s="142"/>
       <c r="C57" s="139" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="D57" s="140"/>
       <c r="E57" s="80">
@@ -5656,7 +5650,7 @@
       <c r="A58" s="1"/>
       <c r="B58" s="142"/>
       <c r="C58" s="139" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="D58" s="140"/>
       <c r="E58" s="80">
@@ -5697,7 +5691,7 @@
       <c r="A59" s="1"/>
       <c r="B59" s="142"/>
       <c r="C59" s="139" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="D59" s="140"/>
       <c r="E59" s="80">
@@ -5738,7 +5732,7 @@
       <c r="A60" s="1"/>
       <c r="B60" s="142"/>
       <c r="C60" s="139" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="D60" s="140"/>
       <c r="E60" s="80">
@@ -5779,7 +5773,7 @@
       <c r="A61" s="1"/>
       <c r="B61" s="142"/>
       <c r="C61" s="139" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="D61" s="140"/>
       <c r="E61" s="80">
@@ -5820,7 +5814,7 @@
       <c r="A62" s="1"/>
       <c r="B62" s="142"/>
       <c r="C62" s="139" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="D62" s="140"/>
       <c r="E62" s="80">
@@ -5861,7 +5855,7 @@
       <c r="A63" s="1"/>
       <c r="B63" s="142"/>
       <c r="C63" s="139" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="D63" s="140"/>
       <c r="E63" s="80">
@@ -5902,7 +5896,7 @@
       <c r="A64" s="1"/>
       <c r="B64" s="142"/>
       <c r="C64" s="139" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="D64" s="140"/>
       <c r="E64" s="80">
@@ -5943,7 +5937,7 @@
       <c r="A65" s="1"/>
       <c r="B65" s="142"/>
       <c r="C65" s="139" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="D65" s="140"/>
       <c r="E65" s="80">
@@ -5984,7 +5978,7 @@
       <c r="A66" s="1"/>
       <c r="B66" s="142"/>
       <c r="C66" s="139" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="D66" s="140"/>
       <c r="E66" s="80">
@@ -6025,7 +6019,7 @@
       <c r="A67" s="1"/>
       <c r="B67" s="142"/>
       <c r="C67" s="139" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="D67" s="140"/>
       <c r="E67" s="80">
@@ -6066,7 +6060,7 @@
       <c r="A68" s="1"/>
       <c r="B68" s="142"/>
       <c r="C68" s="139" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="D68" s="140"/>
       <c r="E68" s="80">
@@ -6107,7 +6101,7 @@
       <c r="A69" s="1"/>
       <c r="B69" s="142"/>
       <c r="C69" s="139" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="D69" s="140"/>
       <c r="E69" s="80">
@@ -6148,7 +6142,7 @@
       <c r="A70" s="1"/>
       <c r="B70" s="142"/>
       <c r="C70" s="139" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="D70" s="140"/>
       <c r="E70" s="80">
@@ -6189,7 +6183,7 @@
       <c r="A71" s="1"/>
       <c r="B71" s="136"/>
       <c r="C71" s="139" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="D71" s="140"/>
       <c r="E71" s="80">
@@ -6229,7 +6223,7 @@
     <row r="72" spans="1:33" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="1"/>
       <c r="B72" s="85" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="C72" s="86"/>
       <c r="D72" s="87"/>
@@ -6247,7 +6241,7 @@
       <c r="L72" s="71"/>
       <c r="M72" s="71"/>
       <c r="N72" s="107" t="s">
-        <v>237</v>
+        <v>242</v>
       </c>
       <c r="O72" s="1"/>
       <c r="P72" s="1"/>
@@ -6272,7 +6266,7 @@
     <row r="73" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
       <c r="B73" s="91" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="C73" s="92">
         <f>SUM(E4:E72)</f>
@@ -6389,7 +6383,7 @@
     <row r="76" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
       <c r="B76" s="95" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C76" s="4"/>
       <c r="D76" s="1"/>
@@ -6426,16 +6420,16 @@
     <row r="77" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
       <c r="B77" s="60" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="C77" s="25" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="D77" s="60" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="E77" s="143" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="F77" s="144"/>
       <c r="G77" s="144"/>
@@ -6443,7 +6437,7 @@
       <c r="I77" s="144"/>
       <c r="J77" s="145"/>
       <c r="K77" s="143" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="L77" s="145"/>
       <c r="M77" s="3"/>
@@ -6474,13 +6468,13 @@
         <v>253</v>
       </c>
       <c r="C78" s="25" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="D78" s="60" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="E78" s="143" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="F78" s="144"/>
       <c r="G78" s="144"/>
@@ -6488,7 +6482,7 @@
       <c r="I78" s="144"/>
       <c r="J78" s="145"/>
       <c r="K78" s="146" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="L78" s="147"/>
       <c r="M78" s="96"/>
@@ -6519,13 +6513,13 @@
         <v>254</v>
       </c>
       <c r="C79" s="25" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="D79" s="60" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="E79" s="143" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="F79" s="144"/>
       <c r="G79" s="144"/>
@@ -6562,13 +6556,13 @@
         <v>255</v>
       </c>
       <c r="C80" s="25" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="D80" s="60" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="E80" s="143" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="F80" s="144"/>
       <c r="G80" s="144"/>
@@ -6605,13 +6599,13 @@
         <v>4093</v>
       </c>
       <c r="C81" s="25" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="D81" s="60" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="E81" s="143" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="F81" s="144"/>
       <c r="G81" s="144"/>
@@ -6648,13 +6642,13 @@
         <v>4094</v>
       </c>
       <c r="C82" s="25" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="D82" s="60" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="E82" s="143" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="F82" s="144"/>
       <c r="G82" s="144"/>
@@ -6691,13 +6685,13 @@
         <v>4095</v>
       </c>
       <c r="C83" s="25" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="D83" s="60" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="E83" s="143" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="F83" s="144"/>
       <c r="G83" s="144"/>
@@ -6760,7 +6754,7 @@
     <row r="85" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
       <c r="B85" s="99" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="C85" s="100"/>
       <c r="D85" s="97"/>

</xml_diff>